<commit_message>
GK: run code arab and palestinians and works
</commit_message>
<xml_diff>
--- a/create_forecast_basic/future/arab_and_palestinian/Intermediates/taz_Arab_Palestinian_2025.xlsx
+++ b/create_forecast_basic/future/arab_and_palestinian/Intermediates/taz_Arab_Palestinian_2025.xlsx
@@ -3121,58 +3121,58 @@
         <v>6801</v>
       </c>
       <c r="B48" t="n">
-        <v>6154.13</v>
+        <v>6154.12</v>
       </c>
       <c r="C48" t="n">
-        <v>32999.67</v>
+        <v>32999.66</v>
       </c>
       <c r="D48" t="n">
-        <v>4289.9571</v>
+        <v>4289.955800000001</v>
       </c>
       <c r="E48" t="n">
-        <v>3629.9637</v>
+        <v>3629.9626</v>
       </c>
       <c r="F48" t="n">
-        <v>3629.9637</v>
+        <v>3629.9626</v>
       </c>
       <c r="G48" t="n">
-        <v>3299.967</v>
+        <v>3299.966</v>
       </c>
       <c r="H48" t="n">
-        <v>2639.9736</v>
+        <v>2639.9728</v>
       </c>
       <c r="I48" t="n">
-        <v>1979.9802</v>
+        <v>1979.9796</v>
       </c>
       <c r="J48" t="n">
-        <v>1649.9835</v>
+        <v>1649.983</v>
       </c>
       <c r="K48" t="n">
-        <v>1649.9835</v>
+        <v>1649.983</v>
       </c>
       <c r="L48" t="n">
-        <v>1649.9835</v>
+        <v>1649.983</v>
       </c>
       <c r="M48" t="n">
-        <v>3629.9637</v>
+        <v>3629.9626</v>
       </c>
       <c r="N48" t="n">
-        <v>1319.9868</v>
+        <v>1319.9864</v>
       </c>
       <c r="O48" t="n">
-        <v>989.9900999999999</v>
+        <v>989.9898000000001</v>
       </c>
       <c r="P48" t="n">
-        <v>989.9900999999999</v>
+        <v>989.9898000000001</v>
       </c>
       <c r="Q48" t="n">
-        <v>659.9934</v>
+        <v>659.9932000000001</v>
       </c>
       <c r="R48" t="n">
-        <v>329.9967</v>
+        <v>329.9966000000001</v>
       </c>
       <c r="S48" t="n">
-        <v>659.9934</v>
+        <v>659.9932000000001</v>
       </c>
     </row>
     <row r="49">
@@ -3888,7 +3888,7 @@
         <v>1204</v>
       </c>
       <c r="B61" t="n">
-        <v>1337.17</v>
+        <v>1337.16</v>
       </c>
       <c r="C61" t="n">
         <v>5462.959999999999</v>
@@ -4653,55 +4653,55 @@
         <v>607.25</v>
       </c>
       <c r="C75" t="n">
-        <v>2321.549999999999</v>
+        <v>2321.539999999999</v>
       </c>
       <c r="D75" t="n">
-        <v>284.2714285714285</v>
+        <v>284.2702040816325</v>
       </c>
       <c r="E75" t="n">
-        <v>213.2035714285714</v>
+        <v>213.2026530612244</v>
       </c>
       <c r="F75" t="n">
-        <v>213.2035714285714</v>
+        <v>213.2026530612244</v>
       </c>
       <c r="G75" t="n">
-        <v>213.2035714285714</v>
+        <v>213.2026530612244</v>
       </c>
       <c r="H75" t="n">
-        <v>213.2035714285714</v>
+        <v>213.2026530612244</v>
       </c>
       <c r="I75" t="n">
-        <v>165.825</v>
+        <v>165.8242857142857</v>
       </c>
       <c r="J75" t="n">
-        <v>118.4464285714286</v>
+        <v>118.4459183673469</v>
       </c>
       <c r="K75" t="n">
-        <v>118.4464285714286</v>
+        <v>118.4459183673469</v>
       </c>
       <c r="L75" t="n">
-        <v>118.4464285714286</v>
+        <v>118.4459183673469</v>
       </c>
       <c r="M75" t="n">
-        <v>236.8928571428571</v>
+        <v>236.8918367346938</v>
       </c>
       <c r="N75" t="n">
-        <v>118.4464285714286</v>
+        <v>118.4459183673469</v>
       </c>
       <c r="O75" t="n">
-        <v>94.75714285714284</v>
+        <v>94.75673469387752</v>
       </c>
       <c r="P75" t="n">
-        <v>71.06785714285712</v>
+        <v>71.06755102040813</v>
       </c>
       <c r="Q75" t="n">
-        <v>47.37857142857142</v>
+        <v>47.37836734693876</v>
       </c>
       <c r="R75" t="n">
-        <v>47.37857142857142</v>
+        <v>47.37836734693876</v>
       </c>
       <c r="S75" t="n">
-        <v>47.37857142857142</v>
+        <v>47.37836734693876</v>
       </c>
     </row>
     <row r="76">
@@ -5299,58 +5299,58 @@
         <v>303</v>
       </c>
       <c r="B86" t="n">
-        <v>463.78</v>
+        <v>460.06</v>
       </c>
       <c r="C86" t="n">
-        <v>2386.999999999999</v>
+        <v>2091.29</v>
       </c>
       <c r="D86" t="n">
-        <v>216.9999999999999</v>
+        <v>190.1172727272727</v>
       </c>
       <c r="E86" t="n">
-        <v>192.8888888888888</v>
+        <v>168.9931313131313</v>
       </c>
       <c r="F86" t="n">
-        <v>168.7777777777778</v>
+        <v>147.8689898989899</v>
       </c>
       <c r="G86" t="n">
-        <v>192.8888888888888</v>
+        <v>168.9931313131313</v>
       </c>
       <c r="H86" t="n">
-        <v>192.8888888888888</v>
+        <v>168.9931313131313</v>
       </c>
       <c r="I86" t="n">
-        <v>144.6666666666666</v>
+        <v>126.7448484848485</v>
       </c>
       <c r="J86" t="n">
-        <v>168.7777777777778</v>
+        <v>147.8689898989899</v>
       </c>
       <c r="K86" t="n">
-        <v>144.6666666666666</v>
+        <v>126.7448484848485</v>
       </c>
       <c r="L86" t="n">
-        <v>144.6666666666666</v>
+        <v>126.7448484848485</v>
       </c>
       <c r="M86" t="n">
-        <v>192.8888888888888</v>
+        <v>168.9931313131313</v>
       </c>
       <c r="N86" t="n">
-        <v>120.5555555555555</v>
+        <v>105.6207070707071</v>
       </c>
       <c r="O86" t="n">
-        <v>120.5555555555555</v>
+        <v>105.6207070707071</v>
       </c>
       <c r="P86" t="n">
-        <v>96.44444444444441</v>
+        <v>84.49656565656564</v>
       </c>
       <c r="Q86" t="n">
-        <v>72.33333333333331</v>
+        <v>63.37242424242423</v>
       </c>
       <c r="R86" t="n">
-        <v>72.33333333333331</v>
+        <v>63.37242424242423</v>
       </c>
       <c r="S86" t="n">
-        <v>144.6666666666666</v>
+        <v>126.7448484848485</v>
       </c>
     </row>
     <row r="87">

</xml_diff>